<commit_message>
Cache timelime for 1 minute because Excel triple-requests it
</commit_message>
<xml_diff>
--- a/t4e.xlsx
+++ b/t4e.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="timeline" localSheetId="0">Sheet1!$A$1:$C$197</definedName>
@@ -20,7 +18,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" interval="15" name="timeline" type="6" refreshedVersion="4" background="1" refreshOnLoad="1">
+  <connection id="1" interval="5" name="timeline" type="6" refreshedVersion="4" background="1" refreshOnLoad="1">
     <textPr prompt="0" sourceFile="http://10.4.4.155:8088/t4e/timeline">
       <textFields count="2">
         <textField/>
@@ -157,7 +155,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="timeline" refreshOnLoad="1" removeDataOnSave="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="timeline" refreshOnLoad="1" growShrinkType="overwriteClear" removeDataOnSave="1" adjustColumnWidth="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,28 +1446,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>